<commit_message>
Minor changes to head array DAC analysis doc
</commit_message>
<xml_diff>
--- a/HeadArray/DAC_Analysis.xlsx
+++ b/HeadArray/DAC_Analysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tpars\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Invacare\ASL110\ASL110_Documentation\HeadArray\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12683B1B-C9F4-48D7-A699-BDFE4EE1B58B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55BF66D6-5AF6-4ECC-9168-C57784C5A26C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5733FAC2-2F46-4B2B-A51C-B52997863F09}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5733FAC2-2F46-4B2B-A51C-B52997863F09}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -76,8 +76,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0.00000"/>
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -156,15 +156,15 @@
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,7 +482,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,12 +505,12 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
       <c r="I2" s="1" t="s">
         <v>10</v>
       </c>
@@ -542,7 +542,7 @@
         <f>ROUND(4.8/0.00295, 0)</f>
         <v>1627</v>
       </c>
-      <c r="J3" s="8">
+      <c r="J3" s="7">
         <f>I3*0.00295</f>
         <v>4.7996499999999997</v>
       </c>
@@ -554,14 +554,14 @@
       <c r="B4">
         <v>0.29199999999999998</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <f>B4/100</f>
         <v>2.9199999999999999E-3</v>
       </c>
       <c r="D4">
         <v>0.29499999999999998</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <f>D4/100</f>
         <v>2.9499999999999999E-3</v>
       </c>
@@ -572,7 +572,7 @@
         <f>ROUND(6/0.00295, 0)</f>
         <v>2034</v>
       </c>
-      <c r="J4" s="8">
+      <c r="J4" s="7">
         <f t="shared" ref="J4:J5" si="0">I4*0.00295</f>
         <v>6.0003000000000002</v>
       </c>
@@ -584,14 +584,14 @@
       <c r="B5">
         <v>0.58599999999999997</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <f>(B5-B4)/(A5-A4)</f>
         <v>2.9399999999999999E-3</v>
       </c>
       <c r="D5">
         <v>0.58899999999999997</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <f>(D5-D4)/(A5-A4)</f>
         <v>2.9399999999999999E-3</v>
       </c>
@@ -602,7 +602,7 @@
         <f>ROUND(7.2/0.00295, 0)</f>
         <v>2441</v>
       </c>
-      <c r="J5" s="8">
+      <c r="J5" s="7">
         <f t="shared" si="0"/>
         <v>7.2009499999999997</v>
       </c>
@@ -614,14 +614,14 @@
       <c r="B6">
         <v>1.4710000000000001</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <f t="shared" ref="C6:C9" si="1">(B6-B5)/(A6-A5)</f>
         <v>2.9500000000000004E-3</v>
       </c>
       <c r="D6">
         <v>1.476</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <f t="shared" ref="E6:E9" si="2">(D6-D5)/(A6-A5)</f>
         <v>2.9566666666666669E-3</v>
       </c>
@@ -633,14 +633,14 @@
       <c r="B7">
         <v>2.952</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <f t="shared" si="1"/>
         <v>2.9619999999999998E-3</v>
       </c>
       <c r="D7">
         <v>2.9540000000000002</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <f t="shared" si="2"/>
         <v>2.9560000000000003E-3</v>
       </c>
@@ -652,14 +652,14 @@
       <c r="B8">
         <v>5.91</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <f t="shared" si="1"/>
         <v>2.9580000000000001E-3</v>
       </c>
       <c r="D8">
         <v>5.9130000000000003</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <f t="shared" si="2"/>
         <v>2.9590000000000003E-3</v>
       </c>
@@ -675,14 +675,14 @@
       <c r="B9">
         <v>7.39</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <f t="shared" si="1"/>
         <v>2.9599999999999991E-3</v>
       </c>
       <c r="D9">
         <v>7.39</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <f t="shared" si="2"/>
         <v>2.9539999999999987E-3</v>
       </c>
@@ -692,16 +692,16 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="6">
+      <c r="B10" s="4"/>
+      <c r="C10" s="5">
         <f>AVERAGE(C4:C9)</f>
         <v>2.9483333333333328E-3</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="7">
+      <c r="D10" s="4"/>
+      <c r="E10" s="6">
         <f>AVERAGE(E4:E9)</f>
         <v>2.9526111111111107E-3</v>
       </c>

</xml_diff>